<commit_message>
Se completa diagrama de flujode gerencia falta definir las responsabilidades
</commit_message>
<xml_diff>
--- a/PapeleriaAcuarela.xlsx
+++ b/PapeleriaAcuarela.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javier\Desktop\mapProcesos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7271A57A-A75D-4F73-854A-B8B9BC16BA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52056347-4DF9-45C9-AFD9-57D8864FEA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="861" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="861" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentacion_Mapa_de_Procesos" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,8 @@
     <definedName name="Print_Titles" localSheetId="4">'Gerencia 1'!$A$1:$F$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Gerencia 1'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -863,12 +864,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\-yy;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1001,7 +1009,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1064,6 +1072,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1950,165 +1964,166 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="60" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="60" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2116,10 +2131,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
@@ -2130,58 +2145,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2192,22 +2207,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2230,48 +2245,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -2282,34 +2297,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="60" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="60" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="45" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="45" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="46" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="46" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2328,7 +2343,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2340,285 +2355,299 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="17" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="59" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="59" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="66" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="63" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="66" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="26" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="63" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="59" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="40% - Énfasis6" xfId="6" builtinId="51"/>
+    <cellStyle name="60% - Énfasis5" xfId="7" builtinId="48"/>
     <cellStyle name="Cálculo" xfId="5" builtinId="22"/>
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4212,7 +4241,7 @@
         </a:prstGeom>
         <a:solidFill>
           <a:schemeClr val="accent1">
-            <a:lumMod val="50000"/>
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
       </xdr:spPr>
@@ -10148,8 +10177,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1133475</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -10166,7 +10195,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="161925"/>
-          <a:ext cx="942975" cy="1762125"/>
+          <a:ext cx="942975" cy="1666875"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
@@ -10205,6 +10234,451 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1990725</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>971550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Elipse 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E696F7A-717C-4B33-ABC0-CC42A0865B98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="876300"/>
+          <a:ext cx="1647825" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
+            <a:t>INICIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2143124</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1247775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo: esquinas redondeadas 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE8906D5-397F-4662-A599-6BC2A547F67C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476499" y="2009774"/>
+          <a:ext cx="1952625" cy="1152526"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>*Analisis del producto en el mercado actual </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>*Tomar una decisiones y llegar a acuerdos con clientes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" baseline="0"/>
+            <a:t> y  proveedores</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1514475</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo: esquinas redondeadas 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{432E98E1-2AE6-439A-9154-995DE248C749}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2495550" y="3524250"/>
+          <a:ext cx="1924050" cy="1343025"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>De acuerdo a los planteamientos</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" baseline="0"/>
+            <a:t> de los ideales se procedera a generar las propuestas publicitarias y proyeccion de produccion</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2162175</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1419224</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectángulo: esquinas redondeadas 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9AD636B-3F0F-40D4-9266-C2C634E6C72B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2486025" y="5200649"/>
+          <a:ext cx="1962150" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t>Establecer las directrices para la empresa en cuanto la prestacion de los recursos, Objetivos estrategicos, politicas corporativas</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" baseline="0"/>
+            <a:t> y</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100"/>
+            <a:t> Estrategias empresariales </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1166812</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>971550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1166813</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector recto de flecha 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4665EC0-1254-4C0E-B233-DD408DF0E884}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="4"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3452812" y="1657350"/>
+          <a:ext cx="1" cy="352424"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1166812</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1247775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1171575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector recto de flecha 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3330D71E-5689-44FF-9785-3DD46A96D4DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3452812" y="3162300"/>
+          <a:ext cx="4763" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1171575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1514475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector recto de flecha 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3984188-F7F3-4817-B6C9-0642D2070B62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="6" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3457575" y="4867275"/>
+          <a:ext cx="9525" cy="333374"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -12145,149 +12619,149 @@
       <c r="K3" s="44"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="199" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="189"/>
-      <c r="C4" s="189"/>
-      <c r="D4" s="189"/>
-      <c r="E4" s="189"/>
-      <c r="F4" s="189"/>
-      <c r="G4" s="189"/>
-      <c r="H4" s="189"/>
-      <c r="I4" s="189"/>
-      <c r="J4" s="189"/>
-      <c r="K4" s="189"/>
+      <c r="B4" s="199"/>
+      <c r="C4" s="199"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="199"/>
+      <c r="F4" s="199"/>
+      <c r="G4" s="199"/>
+      <c r="H4" s="199"/>
+      <c r="I4" s="199"/>
+      <c r="J4" s="199"/>
+      <c r="K4" s="199"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="189"/>
-      <c r="B5" s="189"/>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="189"/>
-      <c r="F5" s="189"/>
-      <c r="G5" s="189"/>
-      <c r="H5" s="189"/>
-      <c r="I5" s="189"/>
-      <c r="J5" s="189"/>
-      <c r="K5" s="189"/>
+      <c r="A5" s="199"/>
+      <c r="B5" s="199"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="199"/>
+      <c r="F5" s="199"/>
+      <c r="G5" s="199"/>
+      <c r="H5" s="199"/>
+      <c r="I5" s="199"/>
+      <c r="J5" s="199"/>
+      <c r="K5" s="199"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="189"/>
-      <c r="B6" s="189"/>
-      <c r="C6" s="189"/>
-      <c r="D6" s="189"/>
-      <c r="E6" s="189"/>
-      <c r="F6" s="189"/>
-      <c r="G6" s="189"/>
-      <c r="H6" s="189"/>
-      <c r="I6" s="189"/>
-      <c r="J6" s="189"/>
-      <c r="K6" s="189"/>
+      <c r="A6" s="199"/>
+      <c r="B6" s="199"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="199"/>
+      <c r="E6" s="199"/>
+      <c r="F6" s="199"/>
+      <c r="G6" s="199"/>
+      <c r="H6" s="199"/>
+      <c r="I6" s="199"/>
+      <c r="J6" s="199"/>
+      <c r="K6" s="199"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="189"/>
-      <c r="B7" s="189"/>
-      <c r="C7" s="189"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="189"/>
-      <c r="F7" s="189"/>
-      <c r="G7" s="189"/>
-      <c r="H7" s="189"/>
-      <c r="I7" s="189"/>
-      <c r="J7" s="189"/>
-      <c r="K7" s="189"/>
+      <c r="A7" s="199"/>
+      <c r="B7" s="199"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="199"/>
+      <c r="E7" s="199"/>
+      <c r="F7" s="199"/>
+      <c r="G7" s="199"/>
+      <c r="H7" s="199"/>
+      <c r="I7" s="199"/>
+      <c r="J7" s="199"/>
+      <c r="K7" s="199"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="190"/>
-      <c r="B8" s="190"/>
-      <c r="C8" s="190"/>
-      <c r="D8" s="190"/>
-      <c r="E8" s="190"/>
-      <c r="F8" s="190"/>
-      <c r="G8" s="190"/>
-      <c r="H8" s="190"/>
-      <c r="I8" s="190"/>
-      <c r="J8" s="190"/>
-      <c r="K8" s="190"/>
+      <c r="A8" s="200"/>
+      <c r="B8" s="200"/>
+      <c r="C8" s="200"/>
+      <c r="D8" s="200"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="200"/>
+      <c r="G8" s="200"/>
+      <c r="H8" s="200"/>
+      <c r="I8" s="200"/>
+      <c r="J8" s="200"/>
+      <c r="K8" s="200"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="190"/>
-      <c r="B9" s="190"/>
-      <c r="C9" s="190"/>
-      <c r="D9" s="190"/>
-      <c r="E9" s="190"/>
-      <c r="F9" s="190"/>
-      <c r="G9" s="190"/>
-      <c r="H9" s="190"/>
-      <c r="I9" s="190"/>
-      <c r="J9" s="190"/>
-      <c r="K9" s="190"/>
+      <c r="A9" s="200"/>
+      <c r="B9" s="200"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="200"/>
+      <c r="K9" s="200"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="190"/>
-      <c r="B10" s="190"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="190"/>
-      <c r="H10" s="190"/>
-      <c r="I10" s="190"/>
-      <c r="J10" s="190"/>
-      <c r="K10" s="190"/>
+      <c r="A10" s="200"/>
+      <c r="B10" s="200"/>
+      <c r="C10" s="200"/>
+      <c r="D10" s="200"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="200"/>
+      <c r="G10" s="200"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="200"/>
+      <c r="J10" s="200"/>
+      <c r="K10" s="200"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="190"/>
-      <c r="B11" s="190"/>
-      <c r="C11" s="190"/>
-      <c r="D11" s="190"/>
-      <c r="E11" s="190"/>
-      <c r="F11" s="190"/>
-      <c r="G11" s="190"/>
-      <c r="H11" s="190"/>
-      <c r="I11" s="190"/>
-      <c r="J11" s="190"/>
-      <c r="K11" s="190"/>
+      <c r="A11" s="200"/>
+      <c r="B11" s="200"/>
+      <c r="C11" s="200"/>
+      <c r="D11" s="200"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="200"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="200"/>
+      <c r="K11" s="200"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="190"/>
-      <c r="B12" s="190"/>
-      <c r="C12" s="190"/>
-      <c r="D12" s="190"/>
-      <c r="E12" s="190"/>
-      <c r="F12" s="190"/>
-      <c r="G12" s="190"/>
-      <c r="H12" s="190"/>
-      <c r="I12" s="190"/>
-      <c r="J12" s="190"/>
-      <c r="K12" s="190"/>
+      <c r="A12" s="200"/>
+      <c r="B12" s="200"/>
+      <c r="C12" s="200"/>
+      <c r="D12" s="200"/>
+      <c r="E12" s="200"/>
+      <c r="F12" s="200"/>
+      <c r="G12" s="200"/>
+      <c r="H12" s="200"/>
+      <c r="I12" s="200"/>
+      <c r="J12" s="200"/>
+      <c r="K12" s="200"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="190"/>
-      <c r="B13" s="190"/>
-      <c r="C13" s="190"/>
-      <c r="D13" s="190"/>
-      <c r="E13" s="190"/>
-      <c r="F13" s="190"/>
-      <c r="G13" s="190"/>
-      <c r="H13" s="190"/>
-      <c r="I13" s="190"/>
-      <c r="J13" s="190"/>
-      <c r="K13" s="190"/>
+      <c r="A13" s="200"/>
+      <c r="B13" s="200"/>
+      <c r="C13" s="200"/>
+      <c r="D13" s="200"/>
+      <c r="E13" s="200"/>
+      <c r="F13" s="200"/>
+      <c r="G13" s="200"/>
+      <c r="H13" s="200"/>
+      <c r="I13" s="200"/>
+      <c r="J13" s="200"/>
+      <c r="K13" s="200"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="190"/>
-      <c r="B14" s="190"/>
-      <c r="C14" s="190"/>
-      <c r="D14" s="190"/>
-      <c r="E14" s="190"/>
-      <c r="F14" s="190"/>
-      <c r="G14" s="190"/>
-      <c r="H14" s="190"/>
-      <c r="I14" s="190"/>
-      <c r="J14" s="190"/>
-      <c r="K14" s="190"/>
+      <c r="A14" s="200"/>
+      <c r="B14" s="200"/>
+      <c r="C14" s="200"/>
+      <c r="D14" s="200"/>
+      <c r="E14" s="200"/>
+      <c r="F14" s="200"/>
+      <c r="G14" s="200"/>
+      <c r="H14" s="200"/>
+      <c r="I14" s="200"/>
+      <c r="J14" s="200"/>
+      <c r="K14" s="200"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="45"/>
@@ -12306,12 +12780,12 @@
       <c r="A16" s="45"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
-      <c r="D16" s="191" t="s">
+      <c r="D16" s="201" t="s">
         <v>213</v>
       </c>
-      <c r="E16" s="191"/>
-      <c r="F16" s="191"/>
-      <c r="G16" s="191"/>
+      <c r="E16" s="201"/>
+      <c r="F16" s="201"/>
+      <c r="G16" s="201"/>
       <c r="H16" s="45"/>
       <c r="I16" s="45"/>
       <c r="J16" s="45"/>
@@ -12323,10 +12797,10 @@
       <c r="C17" s="45"/>
       <c r="D17" s="52"/>
       <c r="E17" s="52"/>
-      <c r="F17" s="192" t="s">
+      <c r="F17" s="202" t="s">
         <v>214</v>
       </c>
-      <c r="G17" s="192"/>
+      <c r="G17" s="202"/>
       <c r="H17" s="45"/>
       <c r="I17" s="45"/>
       <c r="J17" s="45"/>
@@ -12338,8 +12812,8 @@
       <c r="C18" s="45"/>
       <c r="D18" s="52"/>
       <c r="E18" s="52"/>
-      <c r="F18" s="193"/>
-      <c r="G18" s="193"/>
+      <c r="F18" s="203"/>
+      <c r="G18" s="203"/>
       <c r="H18" s="45"/>
       <c r="I18" s="45"/>
       <c r="J18" s="45"/>
@@ -12351,8 +12825,8 @@
       <c r="C19" s="45"/>
       <c r="D19" s="77"/>
       <c r="E19" s="76"/>
-      <c r="F19" s="188"/>
-      <c r="G19" s="188"/>
+      <c r="F19" s="198"/>
+      <c r="G19" s="198"/>
       <c r="H19" s="45"/>
       <c r="I19" s="45"/>
       <c r="J19" s="45"/>
@@ -12579,18 +13053,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="227" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="216"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="229"/>
     </row>
     <row r="2" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="217"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="219"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="232"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="46"/>
@@ -12640,45 +13114,45 @@
       <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="205" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="226" t="s">
+      <c r="B2" s="239" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
     </row>
     <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="208" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
+      <c r="E3" s="208"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="227" t="s">
+      <c r="B4" s="240" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="227"/>
-      <c r="D4" s="227"/>
-      <c r="E4" s="227"/>
+      <c r="C4" s="240"/>
+      <c r="D4" s="240"/>
+      <c r="E4" s="240"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
@@ -12732,20 +13206,20 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="199" t="s">
+      <c r="A8" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="200"/>
-      <c r="C8" s="200"/>
-      <c r="D8" s="200"/>
-      <c r="E8" s="201"/>
+      <c r="B8" s="213"/>
+      <c r="C8" s="213"/>
+      <c r="D8" s="213"/>
+      <c r="E8" s="214"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="202"/>
-      <c r="B9" s="203"/>
-      <c r="C9" s="203"/>
-      <c r="D9" s="203"/>
-      <c r="E9" s="204"/>
+      <c r="A9" s="215"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="217"/>
     </row>
     <row r="10" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
@@ -12782,13 +13256,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="194" t="s">
+      <c r="A12" s="204" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="194"/>
-      <c r="C12" s="194"/>
-      <c r="D12" s="194"/>
-      <c r="E12" s="194"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="204"/>
+      <c r="D12" s="204"/>
+      <c r="E12" s="204"/>
     </row>
     <row r="13" spans="1:5" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
@@ -12855,18 +13329,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="227" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="216"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="229"/>
     </row>
     <row r="2" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="217"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="219"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="232"/>
     </row>
     <row r="3" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="59"/>
@@ -13093,45 +13567,45 @@
       <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="228" t="s">
+      <c r="B1" s="241" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="206" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="229"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="242"/>
     </row>
     <row r="3" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="208" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
+      <c r="E3" s="208"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="227" t="s">
+      <c r="B4" s="240" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="227"/>
-      <c r="D4" s="227"/>
-      <c r="E4" s="227"/>
+      <c r="C4" s="240"/>
+      <c r="D4" s="240"/>
+      <c r="E4" s="240"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="67" t="s">
@@ -13202,20 +13676,20 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="199" t="s">
+      <c r="A9" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="200"/>
-      <c r="C9" s="200"/>
-      <c r="D9" s="200"/>
-      <c r="E9" s="201"/>
+      <c r="B9" s="213"/>
+      <c r="C9" s="213"/>
+      <c r="D9" s="213"/>
+      <c r="E9" s="214"/>
     </row>
     <row r="10" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="202"/>
-      <c r="B10" s="203"/>
-      <c r="C10" s="203"/>
-      <c r="D10" s="203"/>
-      <c r="E10" s="204"/>
+      <c r="A10" s="215"/>
+      <c r="B10" s="216"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="217"/>
     </row>
     <row r="11" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
@@ -13252,13 +13726,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="194" t="s">
+      <c r="A13" s="204" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="194"/>
-      <c r="C13" s="194"/>
-      <c r="D13" s="194"/>
-      <c r="E13" s="194"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="204"/>
+      <c r="D13" s="204"/>
+      <c r="E13" s="204"/>
     </row>
     <row r="14" spans="1:5" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="185" t="s">
@@ -13324,18 +13798,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="230" t="s">
+      <c r="B1" s="243" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="245"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="233"/>
-      <c r="C2" s="234"/>
-      <c r="D2" s="235"/>
-      <c r="E2" s="236"/>
+      <c r="B2" s="246"/>
+      <c r="C2" s="247"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="249"/>
     </row>
     <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="59"/>
@@ -13501,45 +13975,45 @@
       <c r="A1" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="237" t="s">
+      <c r="B1" s="250" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="195"/>
-      <c r="D1" s="238"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="251"/>
       <c r="E1" s="164"/>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="206" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="229"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="242"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="208" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
+      <c r="E3" s="208"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="227" t="s">
+      <c r="B4" s="240" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="227"/>
-      <c r="D4" s="227"/>
-      <c r="E4" s="227"/>
+      <c r="C4" s="240"/>
+      <c r="D4" s="240"/>
+      <c r="E4" s="240"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
@@ -13627,20 +14101,20 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="199" t="s">
+      <c r="A10" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="200"/>
-      <c r="C10" s="200"/>
-      <c r="D10" s="200"/>
-      <c r="E10" s="201"/>
+      <c r="B10" s="213"/>
+      <c r="C10" s="213"/>
+      <c r="D10" s="213"/>
+      <c r="E10" s="214"/>
     </row>
     <row r="11" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="202"/>
-      <c r="B11" s="203"/>
-      <c r="C11" s="203"/>
-      <c r="D11" s="203"/>
-      <c r="E11" s="204"/>
+      <c r="A11" s="215"/>
+      <c r="B11" s="216"/>
+      <c r="C11" s="216"/>
+      <c r="D11" s="216"/>
+      <c r="E11" s="217"/>
     </row>
     <row r="12" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -13677,13 +14151,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="194" t="s">
+      <c r="A14" s="204" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="194"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="194"/>
-      <c r="E14" s="194"/>
+      <c r="B14" s="204"/>
+      <c r="C14" s="204"/>
+      <c r="D14" s="204"/>
+      <c r="E14" s="204"/>
     </row>
     <row r="15" spans="1:5" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -13737,7 +14211,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2139DA-D514-425C-BFFA-4FE7C488F1F7}">
   <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13748,18 +14224,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="239" t="s">
+      <c r="B1" s="252" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="241"/>
+      <c r="C1" s="253"/>
+      <c r="D1" s="253"/>
+      <c r="E1" s="254"/>
     </row>
     <row r="2" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="242"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="244"/>
+      <c r="B2" s="255"/>
+      <c r="C2" s="256"/>
+      <c r="D2" s="256"/>
+      <c r="E2" s="257"/>
     </row>
     <row r="3" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="183"/>
@@ -13860,45 +14336,45 @@
       <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="205" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="206" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="245" t="s">
+      <c r="B3" s="258" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="245"/>
-      <c r="D3" s="245"/>
-      <c r="E3" s="245"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="258"/>
+      <c r="E3" s="258"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="246" t="s">
+      <c r="B4" s="259" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="246"/>
-      <c r="D4" s="246"/>
-      <c r="E4" s="246"/>
+      <c r="C4" s="259"/>
+      <c r="D4" s="259"/>
+      <c r="E4" s="259"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
@@ -13986,20 +14462,20 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="199" t="s">
+      <c r="A10" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="200"/>
-      <c r="C10" s="200"/>
-      <c r="D10" s="200"/>
-      <c r="E10" s="201"/>
+      <c r="B10" s="213"/>
+      <c r="C10" s="213"/>
+      <c r="D10" s="213"/>
+      <c r="E10" s="214"/>
     </row>
     <row r="11" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="202"/>
-      <c r="B11" s="203"/>
-      <c r="C11" s="203"/>
-      <c r="D11" s="203"/>
-      <c r="E11" s="204"/>
+      <c r="A11" s="215"/>
+      <c r="B11" s="216"/>
+      <c r="C11" s="216"/>
+      <c r="D11" s="216"/>
+      <c r="E11" s="217"/>
     </row>
     <row r="12" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -14036,13 +14512,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="194" t="s">
+      <c r="A14" s="204" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="194"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="194"/>
-      <c r="E14" s="194"/>
+      <c r="B14" s="204"/>
+      <c r="C14" s="204"/>
+      <c r="D14" s="204"/>
+      <c r="E14" s="204"/>
     </row>
     <row r="15" spans="1:5" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -14122,18 +14598,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="230" t="s">
+      <c r="B1" s="243" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="245"/>
     </row>
     <row r="2" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="233"/>
-      <c r="C2" s="234"/>
-      <c r="D2" s="234"/>
-      <c r="E2" s="236"/>
+      <c r="B2" s="246"/>
+      <c r="C2" s="247"/>
+      <c r="D2" s="247"/>
+      <c r="E2" s="249"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="46"/>
@@ -14288,7 +14764,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14306,8 +14782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14325,47 +14801,47 @@
       <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="205" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="254"/>
-      <c r="F1" s="249"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="189"/>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="206" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="248"/>
-      <c r="F2" s="247"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="188"/>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="208" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="252"/>
-      <c r="F3" s="247"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
+      <c r="E3" s="209"/>
+      <c r="F3" s="188"/>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="198"/>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="253"/>
-      <c r="F4" s="247"/>
+      <c r="B4" s="210"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="211"/>
+      <c r="F4" s="188"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -14380,10 +14856,10 @@
       <c r="D5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="250" t="s">
+      <c r="E5" s="190" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="249"/>
+      <c r="F5" s="189"/>
     </row>
     <row r="6" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
@@ -14398,10 +14874,10 @@
       <c r="D6" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="251" t="s">
+      <c r="E6" s="191" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="249"/>
+      <c r="F6" s="189"/>
     </row>
     <row r="7" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
@@ -14419,7 +14895,7 @@
       <c r="E7" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="249"/>
+      <c r="F7" s="189"/>
     </row>
     <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
@@ -14437,23 +14913,23 @@
       <c r="E8" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="249"/>
+      <c r="F8" s="189"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="199" t="s">
+      <c r="A9" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="200"/>
-      <c r="C9" s="200"/>
-      <c r="D9" s="200"/>
-      <c r="E9" s="201"/>
+      <c r="B9" s="213"/>
+      <c r="C9" s="213"/>
+      <c r="D9" s="213"/>
+      <c r="E9" s="214"/>
     </row>
     <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="202"/>
-      <c r="B10" s="203"/>
-      <c r="C10" s="203"/>
-      <c r="D10" s="203"/>
-      <c r="E10" s="204"/>
+      <c r="A10" s="215"/>
+      <c r="B10" s="216"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="217"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
@@ -14490,13 +14966,13 @@
       </c>
     </row>
     <row r="13" spans="1:10" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="194" t="s">
+      <c r="A13" s="204" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="194"/>
-      <c r="C13" s="194"/>
-      <c r="D13" s="194"/>
-      <c r="E13" s="194"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="204"/>
+      <c r="D13" s="204"/>
+      <c r="E13" s="204"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
@@ -14516,19 +14992,19 @@
       <c r="I14" s="93"/>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="255" t="s">
+      <c r="A15" s="193" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="256" t="s">
+      <c r="B15" s="194" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="257" t="s">
+      <c r="C15" s="195" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="258">
+      <c r="D15" s="196">
         <v>1</v>
       </c>
-      <c r="E15" s="259"/>
+      <c r="E15" s="197"/>
       <c r="H15" s="97"/>
     </row>
     <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14629,9 +15105,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:E4"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14641,18 +15119,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="205" t="s">
+      <c r="B1" s="218" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="207"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="220"/>
     </row>
     <row r="2" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="208"/>
-      <c r="C2" s="209"/>
-      <c r="D2" s="209"/>
-      <c r="E2" s="210"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="223"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="46"/>
@@ -14660,19 +15138,51 @@
       <c r="D3" s="46"/>
       <c r="E3" s="47"/>
     </row>
-    <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="48" t="s">
+    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="260" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="260" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="260" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="261" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="5" spans="2:5" ht="96.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="263">
+        <v>1</v>
+      </c>
+      <c r="C5" s="132"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="123"/>
+    </row>
+    <row r="6" spans="2:5" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="263">
+        <v>2</v>
+      </c>
+      <c r="C6" s="84"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="55"/>
+    </row>
+    <row r="7" spans="2:5" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="263">
+        <v>3</v>
+      </c>
+      <c r="C7" s="84"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="126"/>
+    </row>
+    <row r="8" spans="2:5" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="264">
+        <v>4</v>
+      </c>
+      <c r="C8" s="262"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14703,43 +15213,43 @@
       <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="205" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="211" t="s">
+      <c r="B2" s="224" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
+      <c r="C2" s="224"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="224"/>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="212" t="s">
+      <c r="B3" s="225" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="212"/>
-      <c r="D3" s="212"/>
-      <c r="E3" s="212"/>
+      <c r="C3" s="225"/>
+      <c r="D3" s="225"/>
+      <c r="E3" s="225"/>
     </row>
     <row r="4" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="198"/>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="198"/>
+      <c r="B4" s="210"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
@@ -14793,20 +15303,20 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="213" t="s">
+      <c r="A8" s="226" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="213"/>
-      <c r="C8" s="213"/>
-      <c r="D8" s="213"/>
-      <c r="E8" s="213"/>
+      <c r="B8" s="226"/>
+      <c r="C8" s="226"/>
+      <c r="D8" s="226"/>
+      <c r="E8" s="226"/>
     </row>
     <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="213"/>
-      <c r="B9" s="213"/>
-      <c r="C9" s="213"/>
-      <c r="D9" s="213"/>
-      <c r="E9" s="213"/>
+      <c r="A9" s="226"/>
+      <c r="B9" s="226"/>
+      <c r="C9" s="226"/>
+      <c r="D9" s="226"/>
+      <c r="E9" s="226"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
@@ -14843,13 +15353,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="194" t="s">
+      <c r="A12" s="204" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="194"/>
-      <c r="C12" s="194"/>
-      <c r="D12" s="194"/>
-      <c r="E12" s="194"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="204"/>
+      <c r="D12" s="204"/>
+      <c r="E12" s="204"/>
     </row>
     <row r="13" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
@@ -14954,18 +15464,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="227" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="216"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="229"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="217"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="219"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="232"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="46"/>
@@ -15136,39 +15646,39 @@
       <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="205" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="211"/>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
+      <c r="B2" s="224"/>
+      <c r="C2" s="224"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="224"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="212"/>
-      <c r="C3" s="212"/>
-      <c r="D3" s="212"/>
-      <c r="E3" s="212"/>
+      <c r="B3" s="225"/>
+      <c r="C3" s="225"/>
+      <c r="D3" s="225"/>
+      <c r="E3" s="225"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="198"/>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="198"/>
+      <c r="B4" s="210"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
@@ -15265,20 +15775,20 @@
       <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="220" t="s">
+      <c r="A17" s="233" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="221"/>
-      <c r="C17" s="221"/>
-      <c r="D17" s="221"/>
-      <c r="E17" s="222"/>
+      <c r="B17" s="234"/>
+      <c r="C17" s="234"/>
+      <c r="D17" s="234"/>
+      <c r="E17" s="235"/>
     </row>
     <row r="18" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="223"/>
-      <c r="B18" s="224"/>
-      <c r="C18" s="224"/>
-      <c r="D18" s="224"/>
-      <c r="E18" s="225"/>
+      <c r="A18" s="236"/>
+      <c r="B18" s="237"/>
+      <c r="C18" s="237"/>
+      <c r="D18" s="237"/>
+      <c r="E18" s="238"/>
     </row>
     <row r="19" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
@@ -15305,13 +15815,13 @@
       <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="194" t="s">
+      <c r="A21" s="204" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="194"/>
-      <c r="C21" s="194"/>
-      <c r="D21" s="194"/>
-      <c r="E21" s="194"/>
+      <c r="B21" s="204"/>
+      <c r="C21" s="204"/>
+      <c r="D21" s="204"/>
+      <c r="E21" s="204"/>
     </row>
     <row r="22" spans="1:5" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">

</xml_diff>

<commit_message>
Actualizavion vista de los enlaces
</commit_message>
<xml_diff>
--- a/PapeleriaAcuarela.xlsx
+++ b/PapeleriaAcuarela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javier\Desktop\mapProcesos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB6A218-5523-4571-8D5D-F978D95DDFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB511BC9-8645-44D4-8962-8B423E1972A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="861" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentacion_Mapa_de_Procesos" sheetId="7" r:id="rId1"/>
@@ -1951,7 +1951,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="265">
+  <cellXfs count="266">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -2621,6 +2621,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Énfasis6" xfId="6" builtinId="51"/>
@@ -2773,7 +2774,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1200"/>
+            <a:rPr lang="es-CO" sz="1200" b="1"/>
             <a:t>PRESENTACION</a:t>
           </a:r>
         </a:p>
@@ -4701,7 +4702,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1100"/>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
             <a:t>ONLINE</a:t>
           </a:r>
         </a:p>
@@ -6776,7 +6777,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1100"/>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
             <a:t>CONTABILIDAD</a:t>
           </a:r>
         </a:p>
@@ -8637,7 +8638,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1100"/>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
             <a:t>COMPRAS</a:t>
           </a:r>
         </a:p>
@@ -10608,7 +10609,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1100"/>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
             <a:t>MISION&amp;VISION</a:t>
           </a:r>
         </a:p>
@@ -13434,7 +13435,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1100"/>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
             <a:t>ORGANIGRAMA</a:t>
           </a:r>
         </a:p>
@@ -16070,7 +16071,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1100"/>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
             <a:t>GERENCIA</a:t>
           </a:r>
         </a:p>
@@ -17409,7 +17410,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1100"/>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
             <a:t>VENTAS</a:t>
           </a:r>
         </a:p>
@@ -19157,7 +19158,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-CO" sz="1100"/>
+            <a:rPr lang="es-CO" sz="1100" b="1"/>
             <a:t>LOGISTICA</a:t>
           </a:r>
         </a:p>
@@ -19625,7 +19626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21376,12 +21377,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
@@ -21789,7 +21790,11 @@
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="265"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -22254,7 +22259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>